<commit_message>
Branh terbaru affan (#36)
* last

* uhuy
</commit_message>
<xml_diff>
--- a/src/assets/Template Excel/Layout_Building.xlsx
+++ b/src/assets/Template Excel/Layout_Building.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TABLE SRI\NEW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Worktools SRI\Frontend\sri_monthly_planning_fe\src\assets\Template Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2843F99-18C2-4EF6-914F-4FDAA11DC245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9C9B0C-E2A3-4E6C-9E91-9C55508501FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6DA0EC4C-990A-47CA-B09E-B24038995E24}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{6DA0EC4C-990A-47CA-B09E-B24038995E24}"/>
   </bookViews>
   <sheets>
     <sheet name="BUILDING" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>BUILDING_ID</t>
   </si>
@@ -47,13 +47,7 @@
     <t>PLANT_ID</t>
   </si>
   <si>
-    <t>GEDUNG A</t>
-  </si>
-  <si>
-    <t>GEDUNG B</t>
-  </si>
-  <si>
-    <t>GEDUNG C</t>
+    <t>NOMOR</t>
   </si>
 </sst>
 </file>
@@ -62,15 +56,6 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -92,8 +77,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,8 +99,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -130,32 +129,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -471,94 +481,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B6DA4D-E0D7-490B-9821-AEDE834B2E5C}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" customWidth="1"/>
+    <col min="4" max="4" width="19.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="4"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="4"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="4"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>